<commit_message>
Update Puskopkar Tambah Koperasi
</commit_message>
<xml_diff>
--- a/assets/template/Template_Saldo_simpanan.xlsx
+++ b/assets/template/Template_Saldo_simpanan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\inkopkar\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334BD212-7295-4454-B683-3B6B05B07C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0A72A7-2021-4B76-8E13-2F2F87F2D63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2E8CD1E3-45E7-4754-8C58-5E9B6364AB8C}"/>
   </bookViews>
@@ -512,7 +512,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,10 +552,12 @@
         <v>6</v>
       </c>
       <c r="D2" s="7">
-        <v>45779</v>
+        <f ca="1">TODAY()</f>
+        <v>45880</v>
       </c>
       <c r="E2" s="7">
-        <v>45779</v>
+        <f ca="1">TODAY()</f>
+        <v>45880</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>2</v>

</xml_diff>